<commit_message>
Ajustes en CU. Ajustes visuales en login/signup
</commit_message>
<xml_diff>
--- a/Casos de Uso - Python.xlsx
+++ b/Casos de Uso - Python.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Desktop\python\ProyectoFinal-Py-Beber\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>Proyecto</t>
   </si>
@@ -324,6 +324,15 @@
   </si>
   <si>
     <t>El videojuego se publica correctamente, y al visualizarlo desde su correspondiente categoría se lo puede ver con una imágen default. Se lo redirige al usuario a una vista en la que se le indica que la carga fue exitosa.</t>
+  </si>
+  <si>
+    <t>Notificaciones</t>
+  </si>
+  <si>
+    <t>El usuario ingresa al apartado de notificaciones</t>
+  </si>
+  <si>
+    <t>Esta vista es una vista fija que le muestra al usuario que no tiene notificaciones</t>
   </si>
 </sst>
 </file>
@@ -331,7 +340,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -498,23 +507,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -523,24 +523,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -566,23 +548,38 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -591,6 +588,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -902,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H427"/>
+  <dimension ref="A1:H428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,67 +935,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="16">
+      <c r="B2" s="31"/>
+      <c r="C2" s="24">
         <v>34655</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1005,934 +1020,955 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="16">
         <v>44955</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="9" t="str">
+      <c r="G7" s="6" t="str">
         <f>IF(E7="","Por Hacer", IF(F7="","En Curso", IF(E7=F7,"Aprobado","Desaprobado")))</f>
         <v>Aprobado</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="17">
         <v>44955</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="9" t="str">
-        <f t="shared" ref="G8:G45" si="0">IF(E8="","Por Hacer", IF(F8="","En Curso", IF(E8=F8,"Aprobado","Desaprobado")))</f>
-        <v>Aprobado</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <f t="shared" ref="A9:A45" si="1">A8+1</f>
+      <c r="G8" s="6" t="str">
+        <f t="shared" ref="G8:G46" si="0">IF(E8="","Por Hacer", IF(F8="","En Curso", IF(E8=F8,"Aprobado","Desaprobado")))</f>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <f t="shared" ref="A9:A46" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="17">
         <v>44955</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="18" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Aprobado</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="G9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="17">
         <v>44955</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="9" t="str">
+      <c r="G10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="17">
         <v>44955</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="18" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="9" t="str">
+      <c r="G11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="18">
         <v>44955</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Aprobado</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="G12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="17">
         <v>44955</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="9" t="str">
+      <c r="G13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="17">
         <v>44955</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="18" t="s">
+      <c r="C14" s="34"/>
+      <c r="D14" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="9" t="str">
+      <c r="G14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="17">
         <v>44955</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="18" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="9" t="str">
+      <c r="G15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="17">
         <v>44955</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="9" t="str">
+      <c r="G16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="17">
         <v>44955</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="18" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="9" t="str">
+      <c r="G17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="6">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="17">
         <v>44955</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="18" t="s">
+      <c r="C18" s="34"/>
+      <c r="D18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Aprobado</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="G18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="17">
         <v>44955</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="34"/>
+      <c r="D19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="9" t="str">
+      <c r="G19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="18">
         <v>44955</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="9" t="str">
+      <c r="G20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="19" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="9" t="str">
+      <c r="G21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Desaprobado</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="6">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="18">
         <v>44955</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="19" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="9" t="str">
+      <c r="G22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="17">
         <v>44955</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="9" t="str">
+      <c r="G23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="18">
         <v>44955</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G24" s="9" t="str">
+      <c r="G24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="6">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="18">
         <v>44955</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G25" s="9" t="str">
+      <c r="G25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="6">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="18">
         <v>44955</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="18" t="s">
+      <c r="C26" s="34"/>
+      <c r="D26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="9" t="str">
+      <c r="G26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="6">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="18">
         <v>44955</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="18" t="s">
+      <c r="C27" s="34"/>
+      <c r="D27" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="9" t="str">
+      <c r="G27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="6">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="18">
         <v>44955</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G28" s="9" t="str">
+      <c r="G28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="6">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="18">
         <v>44955</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="19" t="s">
+      <c r="C29" s="30"/>
+      <c r="D29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="9" t="str">
+      <c r="G29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="6">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="18">
         <v>44955</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="9" t="str">
+      <c r="G30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="6">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="18">
         <v>44955</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="18" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G31" s="9" t="str">
+      <c r="G31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="6">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="18">
         <v>44956</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="9" t="str">
+      <c r="G32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="18">
         <v>44956</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G33" s="9" t="str">
+      <c r="G33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="A34" s="6">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B34" s="18">
         <v>44956</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G34" s="9" t="str">
+      <c r="G34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="6">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="18">
         <v>44956</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="23" t="s">
+      <c r="C35" s="30"/>
+      <c r="D35" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="9" t="str">
+      <c r="G35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="6">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="18">
         <v>44956</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="9" t="str">
+      <c r="G36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="6">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="18">
         <v>44956</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="24" t="s">
+      <c r="C37" s="26"/>
+      <c r="D37" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="G37" s="9" t="str">
+      <c r="G37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="A38" s="6">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="18">
         <v>44956</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="30" t="s">
+      <c r="F38" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="G38" s="9" t="str">
+      <c r="G38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="6">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B39" s="18">
         <v>44956</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="23" t="s">
+      <c r="C39" s="28"/>
+      <c r="D39" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E39" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F39" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="9" t="str">
+      <c r="G39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="6">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B40" s="27">
+      <c r="B40" s="18">
         <v>44956</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="23" t="s">
+      <c r="C40" s="28"/>
+      <c r="D40" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F40" s="30" t="s">
+      <c r="F40" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="9" t="str">
+      <c r="G40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="A41" s="6">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B41" s="27">
+      <c r="B41" s="18">
         <v>44956</v>
       </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="F41" s="30" t="s">
+      <c r="F41" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G41" s="9" t="str">
+      <c r="G41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="A42" s="6">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B42" s="27">
+      <c r="B42" s="18">
         <v>44956</v>
       </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="23" t="s">
+      <c r="C42" s="28"/>
+      <c r="D42" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="F42" s="30" t="s">
+      <c r="F42" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="G42" s="9" t="str">
+      <c r="G42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="6">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B43" s="27">
+      <c r="B43" s="18">
         <v>44956</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="23" t="s">
+      <c r="C43" s="28"/>
+      <c r="D43" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="30" t="s">
+      <c r="F43" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="9" t="str">
+      <c r="G43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Aprobado</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="A44" s="6">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B44" s="27">
+      <c r="B44" s="18">
         <v>44956</v>
       </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="23" t="s">
+      <c r="C44" s="29"/>
+      <c r="D44" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E44" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F44" s="22" t="s">
+      <c r="F44" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G44" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Aprobado</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="G44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B45" s="18">
         <v>44956</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B46" s="18">
+        <v>44956</v>
+      </c>
+      <c r="C46" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D46" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="E46" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="21" t="s">
+      <c r="F46" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G45" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Aprobado</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
+      <c r="G46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprobado</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
@@ -1976,6 +2012,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
+      <c r="C57" s="3"/>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
@@ -3087,19 +3124,22 @@
     <row r="427" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B427" s="1"/>
     </row>
+    <row r="428" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B428" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C44"/>
-    <mergeCell ref="C34:C35"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C44"/>
+    <mergeCell ref="C34:C35"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="C7:C11"/>
     <mergeCell ref="C13:C19"/>
@@ -3108,7 +3148,7 @@
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C30:C31"/>
   </mergeCells>
-  <conditionalFormatting sqref="G7:G45">
+  <conditionalFormatting sqref="G7:G46">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Por Hacer"</formula>
     </cfRule>

</xml_diff>